<commit_message>
adjusted data and the name of the bot
</commit_message>
<xml_diff>
--- a/staffing_info_extended.xlsx
+++ b/staffing_info_extended.xlsx
@@ -1,20 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/okonstantinova/Git/other/internal-chat-bot/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33E4F5CF-9FAD-644B-A115-DE7DEB12E8A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="1340" yWindow="11040" windowWidth="26300" windowHeight="12880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="44">
   <si>
     <t>Name</t>
   </si>
@@ -125,13 +144,34 @@
   </si>
   <si>
     <t>Project K: Cloud Infrastructure, Project F: Go Programming</t>
+  </si>
+  <si>
+    <t>Job Level</t>
+  </si>
+  <si>
+    <t>Analyst</t>
+  </si>
+  <si>
+    <t>Consultant</t>
+  </si>
+  <si>
+    <t>Senior Consultant</t>
+  </si>
+  <si>
+    <t>Manager</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Senior Manager </t>
+  </si>
+  <si>
+    <t>Starting Date Available</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -156,7 +196,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -179,28 +219,51 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -238,7 +301,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -272,6 +335,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -306,9 +370,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -481,14 +546,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="27.5" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" customWidth="1"/>
+    <col min="5" max="5" width="52" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -504,8 +578,14 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -513,7 +593,7 @@
         <v>15</v>
       </c>
       <c r="C2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D2" t="s">
         <v>25</v>
@@ -521,8 +601,15 @@
       <c r="E2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2" s="3">
+        <f ca="1">IF(D2="yes",TODAY(),RANDBETWEEN(DATE(2024,6,30),DATE(2024,9,30)))</f>
+        <v>45441</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -530,7 +617,7 @@
         <v>16</v>
       </c>
       <c r="C3">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D3" t="s">
         <v>26</v>
@@ -538,8 +625,15 @@
       <c r="E3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="F3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G3" s="3">
+        <f t="shared" ref="G3:G11" ca="1" si="0">IF(D3="yes",TODAY(),RANDBETWEEN(DATE(2024,6,30),DATE(2024,9,30)))</f>
+        <v>45549</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -547,7 +641,7 @@
         <v>17</v>
       </c>
       <c r="C4">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D4" t="s">
         <v>25</v>
@@ -555,8 +649,15 @@
       <c r="E4" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="F4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G4" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>45441</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -572,8 +673,15 @@
       <c r="E5" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="F5" t="s">
+        <v>41</v>
+      </c>
+      <c r="G5" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>45441</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -581,7 +689,7 @@
         <v>19</v>
       </c>
       <c r="C6">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D6" t="s">
         <v>26</v>
@@ -589,8 +697,15 @@
       <c r="E6" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="F6" t="s">
+        <v>42</v>
+      </c>
+      <c r="G6" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>45478</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -598,7 +713,7 @@
         <v>20</v>
       </c>
       <c r="C7">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D7" t="s">
         <v>25</v>
@@ -606,8 +721,15 @@
       <c r="E7" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="F7" t="s">
+        <v>38</v>
+      </c>
+      <c r="G7" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>45441</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -615,7 +737,7 @@
         <v>21</v>
       </c>
       <c r="C8">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D8" t="s">
         <v>26</v>
@@ -623,8 +745,15 @@
       <c r="E8" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="F8" t="s">
+        <v>39</v>
+      </c>
+      <c r="G8" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>45505</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -632,7 +761,7 @@
         <v>22</v>
       </c>
       <c r="C9">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D9" t="s">
         <v>25</v>
@@ -640,8 +769,15 @@
       <c r="E9" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="10" spans="1:5">
+      <c r="F9" t="s">
+        <v>40</v>
+      </c>
+      <c r="G9" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>45441</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -657,8 +793,15 @@
       <c r="E10" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="11" spans="1:5">
+      <c r="F10" t="s">
+        <v>41</v>
+      </c>
+      <c r="G10" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>45441</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -666,7 +809,7 @@
         <v>24</v>
       </c>
       <c r="C11">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D11" t="s">
         <v>26</v>
@@ -674,8 +817,16 @@
       <c r="E11" t="s">
         <v>36</v>
       </c>
+      <c r="F11" t="s">
+        <v>42</v>
+      </c>
+      <c r="G11" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>45552</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>